<commit_message>
test de caja negra completado para todos los casos de uso
</commit_message>
<xml_diff>
--- a/docs/test-de-sistema/test-planificado/caja-negra/Clases de equivalencia.xlsx
+++ b/docs/test-de-sistema/test-planificado/caja-negra/Clases de equivalencia.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new-obli\proyecto-grupo-4-olivieri-urreta\docs\test-de-sistema\test-planificado\caja-negra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC62CCF-9770-4530-AFAB-7775AEF414F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3111B379-531D-46EB-A971-739DCC4CB5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#CU 1" sheetId="1" r:id="rId1"/>
     <sheet name="#CU 2" sheetId="2" r:id="rId2"/>
+    <sheet name="#CU 3" sheetId="5" r:id="rId3"/>
+    <sheet name="#CU 4" sheetId="6" r:id="rId4"/>
+    <sheet name="#CU 5" sheetId="7" r:id="rId5"/>
+    <sheet name="#CU 6" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="121">
   <si>
     <t>EJECUCION</t>
   </si>
@@ -282,12 +286,291 @@
   <si>
     <t>Contraseña incorrecta (4)</t>
   </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Mensaje: ¡Bienvenido!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Mensaje: Por favor complete todos los campos</t>
+  </si>
+  <si>
+    <r>
+      <t>1,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Monto correcto (2)</t>
+  </si>
+  <si>
+    <t>Fecha correcta (3)</t>
+  </si>
+  <si>
+    <t>Nombre incorrecto (4)</t>
+  </si>
+  <si>
+    <t>Monto incorrecto (5)</t>
+  </si>
+  <si>
+    <t>Fecha incorrecta/vacia (6)</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>Alquiler</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>03/12/2021</t>
+  </si>
+  <si>
+    <t>Mensaje: Gasto creado con éxito</t>
+  </si>
+  <si>
+    <t>Mensaje: Nombre incompleto</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, 2, 3 </t>
+    </r>
+  </si>
+  <si>
+    <t>Mensaje: Monto incompleto</t>
+  </si>
+  <si>
+    <r>
+      <t>1,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,3</t>
+    </r>
+  </si>
+  <si>
+    <t>Mensaje: Fecha incompleta</t>
+  </si>
+  <si>
+    <r>
+      <t>1,2,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> ya que el sistema no permite ingresarlos errados. </t>
+  </si>
+  <si>
+    <t>Descripcion fue retirado del sistema ya que no lo encontramos necesario,</t>
+  </si>
+  <si>
+    <t>por eso fue retirado del caso de uso. Categoria y Repetir no son verificados</t>
+  </si>
+  <si>
+    <t>Fecha invalida (3)</t>
+  </si>
+  <si>
+    <t>Ingresar fecha</t>
+  </si>
+  <si>
+    <t>Hay gastos en el mes/periodo (1)</t>
+  </si>
+  <si>
+    <t>No gastos en el mes/periodo (2)</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Muestra los gastos del mes</t>
+  </si>
+  <si>
+    <t>Muestra los gastos del mes pero no muestra el total de gastos</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Mensaje: Muestra los gastos del periodo ingresado</t>
+  </si>
+  <si>
+    <t>https://github.com/ORT-FIS-202108/proyecto-grupo-4-olivieri-urreta/issues/42</t>
+  </si>
+  <si>
+    <t>Incompleto</t>
+  </si>
+  <si>
+    <t>https://github.com/ORT-FIS-202108/proyecto-grupo-4-olivieri-urreta/issues/43</t>
+  </si>
+  <si>
+    <t>No existe  campo para ingresar fecha invalida</t>
+  </si>
+  <si>
+    <t>Mensaje: No hay gastos registrados para el mes seleccionado</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>No existe campo para ingresar la fecha</t>
+  </si>
+  <si>
+    <t>Ingresar categoria</t>
+  </si>
+  <si>
+    <t>Hay gastos en esa categoria en el periodo ingresado(1)</t>
+  </si>
+  <si>
+    <t>No hay gastos en esa categoria en el periodo ingresado(2)</t>
+  </si>
+  <si>
+    <t>Categoria válida</t>
+  </si>
+  <si>
+    <t>Muestra los gastos del periodo segun categoria</t>
+  </si>
+  <si>
+    <t>Mensaje: No hay gastos registrados para el periodo  seleccionado</t>
+  </si>
+  <si>
+    <t>No existe la funcion de filtrar por gastos</t>
+  </si>
+  <si>
+    <t>https://github.com/ORT-FIS-202108/proyecto-grupo-4-olivieri-urreta/issues/45</t>
+  </si>
+  <si>
+    <t>Enviar compartir gasto a otro usuario (1)</t>
+  </si>
+  <si>
+    <t>El otro usuario no existe (2)</t>
+  </si>
+  <si>
+    <t>Compartir gasto</t>
+  </si>
+  <si>
+    <t>Email invalido (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria  </t>
+  </si>
+  <si>
+    <t>Email a compartir</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>Mensaje: Email invalido</t>
+  </si>
+  <si>
+    <t>Mensaje: Email no registrado en el sistema</t>
+  </si>
+  <si>
+    <t>Le envia un email al otro usuario para aceptar el gasto</t>
+  </si>
+  <si>
+    <t>No existe la funcion de compartir gastos</t>
+  </si>
+  <si>
+    <t>https://github.com/ORT-FIS-202108/proyecto-grupo-4-olivieri-urreta/issues/24</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -360,8 +643,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,8 +674,14 @@
         <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -458,12 +752,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -502,10 +818,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -516,6 +828,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -757,11 +1104,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -832,7 +1179,7 @@
       <c r="I3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="22" t="s">
         <v>36</v>
       </c>
       <c r="K3" s="11" t="s">
@@ -865,19 +1212,19 @@
       <c r="G4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="22" t="s">
         <v>39</v>
       </c>
       <c r="K4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="22" t="s">
         <v>39</v>
       </c>
       <c r="M4" s="20" t="s">
@@ -902,19 +1249,19 @@
         <v>17</v>
       </c>
       <c r="G5" s="17"/>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="22" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="22" t="s">
         <v>40</v>
       </c>
       <c r="M5" s="20" t="s">
@@ -941,10 +1288,10 @@
       <c r="G6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="24" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -971,26 +1318,26 @@
       <c r="G7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="22" t="s">
         <v>46</v>
       </c>
       <c r="K7" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="22" t="s">
         <v>46</v>
       </c>
       <c r="M7" s="20" t="s">
         <v>38</v>
       </c>
       <c r="N7" s="20"/>
-      <c r="O7" s="29" t="s">
+      <c r="O7" s="27" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1017,7 +1364,7 @@
       <c r="L8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="28" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1067,10 +1414,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:O17"/>
+  <dimension ref="B1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I31:I32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1079,23 +1426,23 @@
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31" customWidth="1"/>
-    <col min="12" max="12" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="68.28515625" customWidth="1"/>
-    <col min="15" max="15" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31" customWidth="1"/>
+    <col min="10" max="10" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="68.28515625" customWidth="1"/>
+    <col min="13" max="13" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="L1" s="22" t="s">
+    <row r="1" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-    </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1109,78 +1456,64 @@
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="29" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="H3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="2:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>8</v>
       </c>
@@ -1193,189 +1526,947 @@
       <c r="E4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="F4" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="20" t="s">
+      <c r="H4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="20"/>
-    </row>
-    <row r="5" spans="2:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="2:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
       <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>17</v>
+      <c r="F5" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="G5" s="17"/>
-      <c r="H5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="20" t="s">
+      <c r="H5" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="20"/>
-    </row>
-    <row r="6" spans="2:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="L5" s="41"/>
+    </row>
+    <row r="6" spans="2:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="21"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="36"/>
+    </row>
+    <row r="7" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E7" s="33"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="38"/>
+    </row>
+    <row r="8" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E8" s="33"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="36"/>
+    </row>
+    <row r="9" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I9" s="19"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+    </row>
+    <row r="10" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I10" s="19"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+    </row>
+    <row r="11" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I11" s="19"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+    </row>
+    <row r="12" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I17" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:L1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{D2C050C8-5DDA-450B-AB15-9927A6DF8865}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8B25DD-C1CF-4C5E-921C-8512A2CAC0EA}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B1:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="30" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" style="30" customWidth="1"/>
+    <col min="5" max="8" width="18.7109375" style="30" customWidth="1"/>
+    <col min="9" max="9" width="56.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31" style="30" customWidth="1"/>
+    <col min="11" max="11" width="37.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="30"/>
+    <col min="13" max="13" width="36.28515625" style="30" customWidth="1"/>
+    <col min="14" max="14" width="58.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="14.42578125" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="20"/>
+      <c r="N5" s="30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="20" t="s">
+      <c r="F6" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="25"/>
+      <c r="I6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="20"/>
-    </row>
-    <row r="7" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="20"/>
-      <c r="O7" s="29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K9" s="19"/>
-    </row>
-    <row r="10" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K11" s="19"/>
-    </row>
-    <row r="12" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K14" s="19"/>
-    </row>
-    <row r="15" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="11:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K17" s="19"/>
+      <c r="M6" s="20"/>
+    </row>
+    <row r="7" spans="2:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="2:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="2:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="2:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="10:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C659078-F656-4761-9EA2-6781B3794197}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B1:L17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="30" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31" style="30" customWidth="1"/>
+    <col min="9" max="9" width="64" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="30"/>
+    <col min="11" max="11" width="68.28515625" style="30" customWidth="1"/>
+    <col min="12" max="12" width="58.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="14"/>
+      <c r="C4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="21"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H17" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC2E569-1398-44C6-8092-57AC347313E0}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B1:L17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31" style="30" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="30"/>
+    <col min="11" max="11" width="68.28515625" style="30" customWidth="1"/>
+    <col min="12" max="12" width="58.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="14"/>
+      <c r="C4" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="21"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H17" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABFD8C7-789F-4320-BF02-D30D5E533149}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31" style="30" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="30"/>
+    <col min="11" max="11" width="68.28515625" style="30" customWidth="1"/>
+    <col min="12" max="12" width="58.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="14"/>
+      <c r="C4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="21"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H17" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" xr:uid="{F41A9DA3-CDF9-4C52-A973-FD21F3102476}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{41CF1EA7-42DD-43DF-A0D8-02C53EFEB8AA}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{D2C050C8-5DDA-450B-AB15-9927A6DF8865}"/>
-    <hyperlink ref="H7" r:id="rId4" xr:uid="{E2513ADA-7A11-4791-92FF-B7C08CCA054C}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{D5AA6B24-2C45-4D3A-A7B1-0B855A66E74C}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{172B58E3-E499-4F63-A54A-98F5A47C5F8F}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{9C4EB5A4-1989-4673-A396-E8108A14B656}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>